<commit_message>
Addition of 12V DC DC supply
</commit_message>
<xml_diff>
--- a/kicad_files/D1 Mini - ESP8266/BOM/RatGDO-OpenSource-D1Mini-ESP8266_BOM_JLCSMT.xlsx
+++ b/kicad_files/D1 Mini - ESP8266/BOM/RatGDO-OpenSource-D1Mini-ESP8266_BOM_JLCSMT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\rat-ratgdo\kicad_files\D1 Mini - ESP8266\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C5A57D-BBB6-4771-986E-156F6351ECDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD41584-BB27-4733-A14B-78A20444925D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Comment</t>
   </si>
@@ -31,44 +31,6 @@
     <t>Footprint</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFAFABAB"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>JLCPCB Part #</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFAFABAB"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFAFABAB"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>optional</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFAFABAB"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>）</t>
-    </r>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -93,12 +55,6 @@
     <t>J2</t>
   </si>
   <si>
-    <t>PinHeader_1x10_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>SOT-23</t>
-  </si>
-  <si>
     <t>D_SOD-323_HandSoldering</t>
   </si>
   <si>
@@ -108,9 +64,6 @@
     <t>WEMOS_D1_mini_light</t>
   </si>
   <si>
-    <t>Conn_01x10</t>
-  </si>
-  <si>
     <t>2N7002</t>
   </si>
   <si>
@@ -153,10 +106,64 @@
     <t>C474904</t>
   </si>
   <si>
-    <t>C492409</t>
-  </si>
-  <si>
     <t>C474905</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>B5819W</t>
+  </si>
+  <si>
+    <t>D_SOD-123</t>
+  </si>
+  <si>
+    <t>Converter_DCDC_RECOM_R-78HB-0.5_THT</t>
+  </si>
+  <si>
+    <t>K7805-500R3</t>
+  </si>
+  <si>
+    <t>C_0805_2012Metric_Pad1.18x1.45mm_HandSolder</t>
+  </si>
+  <si>
+    <t>10uF/50V</t>
+  </si>
+  <si>
+    <t>22uF/10V</t>
+  </si>
+  <si>
+    <t>SOT-23_Handsoldering</t>
+  </si>
+  <si>
+    <t>JLCPCB Part #（optional）</t>
+  </si>
+  <si>
+    <t>PinHeader_1x11_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>Conn_01x11</t>
+  </si>
+  <si>
+    <t>C64885</t>
+  </si>
+  <si>
+    <t>C909662</t>
+  </si>
+  <si>
+    <t>C440198</t>
+  </si>
+  <si>
+    <t>C45783</t>
   </si>
 </sst>
 </file>
@@ -177,26 +184,27 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
       <color rgb="FFAFABAB"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFAFABAB"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -210,7 +218,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -218,28 +226,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -249,20 +242,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="20" customHeight="1"/>
@@ -621,129 +623,196 @@
     <col min="4" max="4" width="24.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20" customHeight="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" ht="20" customHeight="1">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="C3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="20" customHeight="1">
+      <c r="A9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="20" customHeight="1">
+      <c r="A10" s="8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="B10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="20" customHeight="1">
+      <c r="A11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
-      <c r="A6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
-      <c r="A8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="C11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" ht="20" customHeight="1">
+      <c r="A12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" ht="20" customHeight="1">
+      <c r="A13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="20" customHeight="1">
-      <c r="A9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="C13" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>